<commit_message>
made some changes on the dashboard
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://kenbright-my.sharepoint.com/personal/rochieng_kenbright_africa/Documents/Attachments/projects/2024/July/Life Insurers in Africa Shiny Dashboard/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="276" documentId="8_{91A81E83-C47E-4463-952B-79D6AAFE2308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9424A3BB-4D2D-4ACA-938E-B55350AAC066}"/>
+  <xr:revisionPtr revIDLastSave="278" documentId="8_{91A81E83-C47E-4463-952B-79D6AAFE2308}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EDD10DA4-1A55-437C-B41C-E153F579A487}"/>
   <bookViews>
-    <workbookView xWindow="2280" yWindow="720" windowWidth="9780" windowHeight="10080" xr2:uid="{290A6BD8-1E2E-4925-A693-0DA480B8D71A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{290A6BD8-1E2E-4925-A693-0DA480B8D71A}"/>
   </bookViews>
   <sheets>
     <sheet name="Insurers" sheetId="1" r:id="rId1"/>
@@ -1592,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D156184C-29D5-4B3B-9A0B-8D2EB0C4ED5C}">
   <dimension ref="A1:F230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>